<commit_message>
xlxs yield title to camel case
</commit_message>
<xml_diff>
--- a/CaliforniaAlmondTracker.xlsx
+++ b/CaliforniaAlmondTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarte\Documents\Github\CMPLXSYS530\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F91834-4966-411F-B5B5-04217F62759C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEB7111-633F-4A04-A63B-DAD311EB475D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3264" yWindow="3264" windowWidth="17280" windowHeight="10074" xr2:uid="{924722FB-807A-4015-AC81-44A9D46CA5FA}"/>
+    <workbookView xWindow="3732" yWindow="1350" windowWidth="17280" windowHeight="10074" xr2:uid="{924722FB-807A-4015-AC81-44A9D46CA5FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -565,10 +565,10 @@
     <t>Gross Value ($1,000)</t>
   </si>
   <si>
-    <t>Almond Yield (tons/ac)</t>
-  </si>
-  <si>
     <t>unit price:</t>
+  </si>
+  <si>
+    <t>almondYield</t>
   </si>
 </sst>
 </file>
@@ -964,7 +964,7 @@
     <col min="17" max="18" width="8.83984375" customWidth="1"/>
     <col min="19" max="19" width="13.68359375" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.15625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
@@ -1029,10 +1029,10 @@
         <v>175</v>
       </c>
       <c r="U1" t="s">
+        <v>177</v>
+      </c>
+      <c r="V1" t="s">
         <v>176</v>
-      </c>
-      <c r="V1" t="s">
-        <v>177</v>
       </c>
       <c r="W1">
         <v>2.4300000000000002</v>

</xml_diff>

<commit_message>
Fire Probability reassigned to reborn nodes
XLXS files : fire probability titles condensed and camel case

python: position was being reassigned and now selects which model of fire probability is being used ('fire mode' - predicted vs observed)
</commit_message>
<xml_diff>
--- a/CaliforniaAlmondTracker.xlsx
+++ b/CaliforniaAlmondTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarte\Documents\Github\CMPLXSYS530\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEB7111-633F-4A04-A63B-DAD311EB475D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9139124-5C71-477A-BCB2-CA94BCD1BD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="1350" windowWidth="17280" windowHeight="10074" xr2:uid="{924722FB-807A-4015-AC81-44A9D46CA5FA}"/>
+    <workbookView xWindow="4068" yWindow="1686" windowWidth="17280" windowHeight="10074" xr2:uid="{924722FB-807A-4015-AC81-44A9D46CA5FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,12 +70,6 @@
     <t>borders</t>
   </si>
   <si>
-    <t>Predicted Fire Prob</t>
-  </si>
-  <si>
-    <t>Observed Fire Prob</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -569,6 +563,12 @@
   </si>
   <si>
     <t>almondYield</t>
+  </si>
+  <si>
+    <t>ObservedfireProb</t>
+  </si>
+  <si>
+    <t>PredictedfireProb</t>
   </si>
 </sst>
 </file>
@@ -948,7 +948,7 @@
   <dimension ref="A1:AC178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScale="91" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1011,28 +1011,28 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
       <c r="S1" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="T1" t="s">
+        <v>173</v>
+      </c>
+      <c r="U1" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1" t="s">
         <v>174</v>
-      </c>
-      <c r="T1" t="s">
-        <v>175</v>
-      </c>
-      <c r="U1" t="s">
-        <v>177</v>
-      </c>
-      <c r="V1" t="s">
-        <v>176</v>
       </c>
       <c r="W1">
         <v>2.4300000000000002</v>
@@ -1046,16 +1046,16 @@
         <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>6001</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3">
         <v>1510271</v>
@@ -1079,7 +1079,7 @@
         <v>821.32799999999997</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O2" s="2">
         <v>1E-3</v>
@@ -1111,16 +1111,16 @@
         <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>6003</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" s="3">
         <v>1175</v>
@@ -1144,7 +1144,7 @@
         <v>743.18</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O3" s="2">
         <v>2.01E-2</v>
@@ -1177,16 +1177,16 @@
         <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>6005</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="3">
         <v>38091</v>
@@ -1210,7 +1210,7 @@
         <v>605.95600000000002</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O4" s="2">
         <v>5.1000000000000004E-3</v>
@@ -1243,16 +1243,16 @@
         <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>6007</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="3">
         <v>220000</v>
@@ -1276,7 +1276,7 @@
         <v>1677.1310000000001</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O5" s="2">
         <v>5.1000000000000004E-3</v>
@@ -1310,16 +1310,16 @@
         <v>191</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>6009</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3">
         <v>45578</v>
@@ -1343,7 +1343,7 @@
         <v>1036.9269999999999</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O6" s="2">
         <v>1.5100000000000001E-2</v>
@@ -1377,16 +1377,16 @@
         <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>6011</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G7" s="3">
         <v>21419</v>
@@ -1410,7 +1410,7 @@
         <v>1156.3610000000001</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O7" s="2">
         <v>0.03</v>
@@ -1444,16 +1444,16 @@
         <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>6013</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G8" s="3">
         <v>1049025</v>
@@ -1477,7 +1477,7 @@
         <v>803.77</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O8" s="2">
         <v>1E-3</v>
@@ -1511,16 +1511,16 @@
         <v>194</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>6015</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3">
         <v>28610</v>
@@ -1544,7 +1544,7 @@
         <v>1229.7429999999999</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O9" s="2">
         <v>1E-3</v>
@@ -1578,16 +1578,16 @@
         <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>6017</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" s="3">
         <v>181058</v>
@@ -1611,7 +1611,7 @@
         <v>1786.356</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O10" s="2">
         <v>1.5100000000000001E-2</v>
@@ -1643,16 +1643,16 @@
         <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>6019</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" s="3">
         <v>930450</v>
@@ -1676,7 +1676,7 @@
         <v>6011.2020000000002</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O11" s="2">
         <v>2.01E-2</v>
@@ -1710,16 +1710,16 @@
         <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>6021</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" s="3">
         <v>28122</v>
@@ -1743,7 +1743,7 @@
         <v>1326.9780000000001</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O12" s="2">
         <v>5.1000000000000004E-3</v>
@@ -1777,16 +1777,16 @@
         <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>6023</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G13" s="3">
         <v>134623</v>
@@ -1810,7 +1810,7 @@
         <v>4052.2579999999998</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O13" s="2">
         <v>5.0000000000000001E-3</v>
@@ -1842,16 +1842,16 @@
         <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>6025</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G14" s="3">
         <v>174528</v>
@@ -1875,7 +1875,7 @@
         <v>4481.7190000000001</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O14" s="2">
         <v>1E-3</v>
@@ -1907,16 +1907,16 @@
         <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>6027</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G15" s="3">
         <v>18546</v>
@@ -1940,7 +1940,7 @@
         <v>10226.905000000001</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O15" s="2">
         <v>1.1000000000000001E-3</v>
@@ -1972,16 +1972,16 @@
         <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>6029</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G16" s="3">
         <v>839631</v>
@@ -2005,7 +2005,7 @@
         <v>8162.6409999999996</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O16" s="2">
         <v>5.1000000000000004E-3</v>
@@ -2038,16 +2038,16 @@
         <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>6031</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G17" s="3">
         <v>152982</v>
@@ -2071,7 +2071,7 @@
         <v>1391.5309999999999</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O17" s="2">
         <v>5.1000000000000004E-3</v>
@@ -2104,16 +2104,16 @@
         <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>6033</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G18" s="3">
         <v>64665</v>
@@ -2137,7 +2137,7 @@
         <v>1329.423</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O18" s="2">
         <v>0.03</v>
@@ -2169,16 +2169,16 @@
         <v>204</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>6035</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G19" s="3">
         <v>34895</v>
@@ -2202,7 +2202,7 @@
         <v>4720.1189999999997</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O19" s="2">
         <v>2.1000000000000001E-2</v>
@@ -2234,16 +2234,16 @@
         <v>205</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>6037</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G20" s="3">
         <v>9818605</v>
@@ -2267,7 +2267,7 @@
         <v>4750.942</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O20" s="2">
         <v>0.03</v>
@@ -2299,16 +2299,16 @@
         <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>6039</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" s="3">
         <v>150865</v>
@@ -2332,7 +2332,7 @@
         <v>2153.2689999999998</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O21" s="2">
         <v>1.0999999999999999E-2</v>
@@ -2365,16 +2365,16 @@
         <v>207</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>6041</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G22" s="3">
         <v>252409</v>
@@ -2398,7 +2398,7 @@
         <v>828.19200000000001</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O22" s="2">
         <v>1E-3</v>
@@ -2430,16 +2430,16 @@
         <v>208</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23">
         <v>6043</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G23" s="3">
         <v>18251</v>
@@ -2463,7 +2463,7 @@
         <v>1462.82</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O23" s="2">
         <v>1.5100000000000001E-2</v>
@@ -2495,16 +2495,16 @@
         <v>209</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24">
         <v>6045</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G24" s="3">
         <v>87841</v>
@@ -2528,7 +2528,7 @@
         <v>3878.1410000000001</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O24" s="2">
         <v>1.5100000000000001E-2</v>
@@ -2560,16 +2560,16 @@
         <v>210</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D25">
         <v>6047</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3">
         <v>255793</v>
@@ -2593,7 +2593,7 @@
         <v>1978.509</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O25" s="2">
         <v>5.1000000000000004E-3</v>
@@ -2626,16 +2626,16 @@
         <v>211</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D26">
         <v>6049</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G26" s="3">
         <v>9686</v>
@@ -2659,7 +2659,7 @@
         <v>4203.3990000000003</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O26" s="2">
         <v>1.4999999999999999E-2</v>
@@ -2691,16 +2691,16 @@
         <v>212</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D27">
         <v>6051</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G27" s="3">
         <v>14202</v>
@@ -2724,7 +2724,7 @@
         <v>3131.8760000000002</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O27" s="2">
         <v>5.1000000000000004E-3</v>
@@ -2756,16 +2756,16 @@
         <v>213</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>6053</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G28" s="3">
         <v>415057</v>
@@ -2789,7 +2789,7 @@
         <v>3771.221</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O28" s="2">
         <v>0.03</v>
@@ -2821,16 +2821,16 @@
         <v>214</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D29">
         <v>6055</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G29" s="3">
         <v>136484</v>
@@ -2854,7 +2854,7 @@
         <v>788.58199999999999</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O29" s="2">
         <v>0.03</v>
@@ -2886,16 +2886,16 @@
         <v>215</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D30">
         <v>6057</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G30" s="3">
         <v>98764</v>
@@ -2919,7 +2919,7 @@
         <v>973.80100000000004</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O30" s="2">
         <v>1.0999999999999999E-2</v>
@@ -2951,16 +2951,16 @@
         <v>216</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D31">
         <v>6059</v>
       </c>
       <c r="E31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G31" s="3">
         <v>3010232</v>
@@ -2984,7 +2984,7 @@
         <v>948.06600000000003</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O31" s="2">
         <v>0.03</v>
@@ -3017,16 +3017,16 @@
         <v>217</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D32">
         <v>6061</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G32" s="3">
         <v>348432</v>
@@ -3050,7 +3050,7 @@
         <v>1502.4559999999999</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O32" s="2">
         <v>0.03</v>
@@ -3084,16 +3084,16 @@
         <v>218</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>6063</v>
       </c>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G33" s="3">
         <v>20007</v>
@@ -3117,7 +3117,7 @@
         <v>2613.4279999999999</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O33" s="2">
         <v>1.1000000000000001E-3</v>
@@ -3150,16 +3150,16 @@
         <v>219</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D34">
         <v>6065</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G34" s="3">
         <v>2189641</v>
@@ -3183,7 +3183,7 @@
         <v>7303.42</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O34" s="2">
         <v>0.03</v>
@@ -3216,16 +3216,16 @@
         <v>220</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D35">
         <v>6067</v>
       </c>
       <c r="E35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G35" s="3">
         <v>1418788</v>
@@ -3249,7 +3249,7 @@
         <v>994.01800000000003</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O35" s="2">
         <v>5.1000000000000004E-3</v>
@@ -3284,16 +3284,16 @@
         <v>221</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D36">
         <v>6069</v>
       </c>
       <c r="E36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G36" s="3">
         <v>55269</v>
@@ -3317,7 +3317,7 @@
         <v>1390.4690000000001</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O36" s="2">
         <v>0.03</v>
@@ -3350,16 +3350,16 @@
         <v>222</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D37">
         <v>6071</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G37" s="3">
         <v>2035210</v>
@@ -3383,7 +3383,7 @@
         <v>20104.826000000001</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O37" s="2">
         <v>0.03</v>
@@ -3416,16 +3416,16 @@
         <v>223</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D38">
         <v>6073</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G38" s="3">
         <v>3095313</v>
@@ -3449,7 +3449,7 @@
         <v>4525.6850000000004</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O38" s="2">
         <v>0.03</v>
@@ -3482,16 +3482,16 @@
         <v>224</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D39">
         <v>6075</v>
       </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G39" s="3">
         <v>805235</v>
@@ -3515,7 +3515,7 @@
         <v>231.88900000000001</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O39" s="2">
         <v>1E-3</v>
@@ -3548,16 +3548,16 @@
         <v>225</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D40">
         <v>6077</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G40" s="3">
         <v>685306</v>
@@ -3581,7 +3581,7 @@
         <v>1426.499</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O40" s="2">
         <v>1.1000000000000001E-3</v>
@@ -3615,16 +3615,16 @@
         <v>226</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D41">
         <v>6079</v>
       </c>
       <c r="E41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G41" s="3">
         <v>269637</v>
@@ -3648,7 +3648,7 @@
         <v>3615.547</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O41" s="2">
         <v>0.03</v>
@@ -3680,16 +3680,16 @@
         <v>227</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D42">
         <v>6081</v>
       </c>
       <c r="E42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G42" s="3">
         <v>718451</v>
@@ -3713,7 +3713,7 @@
         <v>740.95899999999995</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O42" s="2">
         <v>1.4999999999999999E-2</v>
@@ -3745,16 +3745,16 @@
         <v>228</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D43">
         <v>6083</v>
       </c>
       <c r="E43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G43" s="3">
         <v>423895</v>
@@ -3778,7 +3778,7 @@
         <v>3789.078</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O43" s="2">
         <v>0.03</v>
@@ -3810,16 +3810,16 @@
         <v>229</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D44">
         <v>6085</v>
       </c>
       <c r="E44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G44" s="3">
         <v>1781642</v>
@@ -3843,7 +3843,7 @@
         <v>1304.067</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O44" s="2">
         <v>5.1000000000000004E-3</v>
@@ -3875,16 +3875,16 @@
         <v>230</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D45">
         <v>6087</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G45" s="3">
         <v>262382</v>
@@ -3908,7 +3908,7 @@
         <v>607.16600000000005</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O45" s="2">
         <v>1.1000000000000001E-3</v>
@@ -3940,16 +3940,16 @@
         <v>231</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D46">
         <v>6089</v>
       </c>
       <c r="E46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G46" s="3">
         <v>177223</v>
@@ -3973,7 +3973,7 @@
         <v>3847.422</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="O46" s="2">
         <v>0.03</v>
@@ -4006,16 +4006,16 @@
         <v>232</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D47">
         <v>6091</v>
       </c>
       <c r="E47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G47" s="3">
         <v>3240</v>
@@ -4039,7 +4039,7 @@
         <v>962.21</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O47" s="2">
         <v>1.1000000000000001E-3</v>
@@ -4072,16 +4072,16 @@
         <v>233</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D48">
         <v>6093</v>
       </c>
       <c r="E48" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G48" s="3">
         <v>44900</v>
@@ -4105,7 +4105,7 @@
         <v>6347.3429999999998</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="O48" s="2">
         <v>0.03</v>
@@ -4137,16 +4137,16 @@
         <v>234</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D49">
         <v>6095</v>
       </c>
       <c r="E49" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G49" s="3">
         <v>413344</v>
@@ -4170,7 +4170,7 @@
         <v>906.19200000000001</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O49" s="2">
         <v>1E-3</v>
@@ -4204,16 +4204,16 @@
         <v>235</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D50">
         <v>6097</v>
       </c>
       <c r="E50" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F50" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G50" s="3">
         <v>483878</v>
@@ -4237,7 +4237,7 @@
         <v>1767.9469999999999</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O50" s="2">
         <v>1E-3</v>
@@ -4269,16 +4269,16 @@
         <v>236</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D51">
         <v>6099</v>
       </c>
       <c r="E51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G51" s="3">
         <v>514453</v>
@@ -4302,7 +4302,7 @@
         <v>1514.6869999999999</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O51" s="2">
         <v>5.1000000000000004E-3</v>
@@ -4335,16 +4335,16 @@
         <v>237</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D52">
         <v>6101</v>
       </c>
       <c r="E52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G52" s="3">
         <v>94737</v>
@@ -4368,7 +4368,7 @@
         <v>608.49</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O52" s="2">
         <v>1E-3</v>
@@ -4401,16 +4401,16 @@
         <v>238</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D53">
         <v>6103</v>
       </c>
       <c r="E53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G53" s="3">
         <v>63463</v>
@@ -4434,7 +4434,7 @@
         <v>2962.1709999999998</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O53" s="2">
         <v>0.03</v>
@@ -4468,16 +4468,16 @@
         <v>239</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D54">
         <v>6105</v>
       </c>
       <c r="E54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G54" s="3">
         <v>13786</v>
@@ -4501,7 +4501,7 @@
         <v>3207.5970000000002</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O54" s="2">
         <v>0.03</v>
@@ -4534,16 +4534,16 @@
         <v>240</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D55">
         <v>6107</v>
       </c>
       <c r="E55" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F55" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G55" s="3">
         <v>442179</v>
@@ -4567,7 +4567,7 @@
         <v>4838.652</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O55" s="2">
         <v>0.03</v>
@@ -4600,16 +4600,16 @@
         <v>241</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D56">
         <v>6109</v>
       </c>
       <c r="E56" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F56" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G56" s="3">
         <v>55365</v>
@@ -4633,7 +4633,7 @@
         <v>2274.4299999999998</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O56" s="2">
         <v>2.01E-2</v>
@@ -4665,16 +4665,16 @@
         <v>242</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D57">
         <v>6111</v>
       </c>
       <c r="E57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G57" s="3">
         <v>823318</v>
@@ -4698,7 +4698,7 @@
         <v>2208.3820000000001</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="O57" s="2">
         <v>0.03</v>
@@ -4730,16 +4730,16 @@
         <v>243</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D58">
         <v>6113</v>
       </c>
       <c r="E58" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F58" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G58" s="3">
         <v>200849</v>
@@ -4763,7 +4763,7 @@
         <v>1023.557</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O58" s="2">
         <v>0.03</v>
@@ -4796,16 +4796,16 @@
         <v>244</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D59">
         <v>6115</v>
       </c>
       <c r="E59" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G59" s="3">
         <v>72155</v>
@@ -4829,7 +4829,7 @@
         <v>643.80799999999999</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="O59" s="2">
         <v>1.5100000000000001E-2</v>

</xml_diff>

<commit_message>
convert to almond tracking
include almond output of county by ton
</commit_message>
<xml_diff>
--- a/CaliforniaAlmondTracker.xlsx
+++ b/CaliforniaAlmondTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarte\Documents\Github\CMPLXSYS530\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9139124-5C71-477A-BCB2-CA94BCD1BD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6FE83B-3306-42F9-950F-EBF3319041D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4068" yWindow="1686" windowWidth="17280" windowHeight="10074" xr2:uid="{924722FB-807A-4015-AC81-44A9D46CA5FA}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{924722FB-807A-4015-AC81-44A9D46CA5FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="179">
   <si>
     <t>Node</t>
   </si>
@@ -569,6 +569,9 @@
   </si>
   <si>
     <t>PredictedfireProb</t>
+  </si>
+  <si>
+    <t>almondOutput</t>
   </si>
 </sst>
 </file>
@@ -945,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B440007F-2E4E-4D43-9BA3-FF6B61B8A80B}">
-  <dimension ref="A1:AC178"/>
+  <dimension ref="A1:AD178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScale="91" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -964,10 +967,11 @@
     <col min="17" max="18" width="8.83984375" customWidth="1"/>
     <col min="19" max="19" width="13.68359375" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.578125" customWidth="1"/>
+    <col min="22" max="22" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1029,16 +1033,20 @@
         <v>173</v>
       </c>
       <c r="U1" t="s">
+        <v>178</v>
+      </c>
+      <c r="V1" t="s">
         <v>175</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>174</v>
       </c>
-      <c r="W1">
+      <c r="X1">
+        <f>2.43</f>
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1099,11 +1107,15 @@
       <c r="T2">
         <v>0</v>
       </c>
-      <c r="U2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U2">
+        <f>$T2/($X$1*2000)</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1164,12 +1176,16 @@
       <c r="T3">
         <v>0</v>
       </c>
-      <c r="U3" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U3">
+        <f t="shared" ref="U3:U59" si="0">$T3/($X$1*2000)</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1230,12 +1246,16 @@
       <c r="T4">
         <v>0</v>
       </c>
-      <c r="U4" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1296,13 +1316,17 @@
       <c r="T5" s="3">
         <v>147413</v>
       </c>
-      <c r="U5" s="7">
-        <f>($T5*1000*$W$1)/(S5*2000)</f>
-        <v>5.7974621285686538</v>
-      </c>
-      <c r="Z5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>30.331893004115226</v>
+      </c>
+      <c r="V5" s="7">
+        <f>($T5/(S5*2))*(1/$X$1)</f>
+        <v>0.98180530213359296</v>
+      </c>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1363,13 +1387,17 @@
       <c r="T6">
         <v>42</v>
       </c>
-      <c r="U6" s="7">
-        <f t="shared" ref="U6:U59" si="0">($T6*1000*$W$1)/(S6*2000)</f>
-        <v>0.25903553299492388</v>
-      </c>
-      <c r="Z6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>8.6419753086419745E-3</v>
+      </c>
+      <c r="V6" s="7">
+        <f t="shared" ref="V6:V59" si="1">($T6/(S6*2))*(1/$X$1)</f>
+        <v>4.3867894967725758E-2</v>
+      </c>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1430,13 +1458,17 @@
       <c r="T7" s="3">
         <v>307689</v>
       </c>
-      <c r="U7" s="7">
-        <f t="shared" si="0"/>
-        <v>8.022707734237521</v>
-      </c>
-      <c r="Z7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>63.310493827160492</v>
+      </c>
+      <c r="V7" s="7">
+        <f>($T7/(S7*2))*(1/$X$1)</f>
+        <v>1.3586525994068521</v>
+      </c>
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1497,13 +1529,17 @@
       <c r="T8">
         <v>0</v>
       </c>
-      <c r="U8" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1564,13 +1600,17 @@
       <c r="T9" s="3">
         <v>0</v>
       </c>
-      <c r="U9" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="3"/>
-      <c r="AC9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3"/>
+      <c r="AD9" s="3"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1631,11 +1671,15 @@
       <c r="T10">
         <v>0</v>
       </c>
-      <c r="U10" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1696,13 +1740,17 @@
       <c r="T11" s="3">
         <v>1197592</v>
       </c>
-      <c r="U11" s="7">
-        <f t="shared" si="0"/>
-        <v>8.6717896945063586</v>
-      </c>
-      <c r="Z11" s="3"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>246.41810699588478</v>
+      </c>
+      <c r="V11" s="7">
+        <f t="shared" si="1"/>
+        <v>1.4685751993270604</v>
+      </c>
+      <c r="AA11" s="3"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1763,13 +1811,17 @@
       <c r="T12" s="3">
         <v>210466</v>
       </c>
-      <c r="U12" s="7">
-        <f t="shared" si="0"/>
-        <v>7.4864944228123091</v>
-      </c>
-      <c r="Z12" s="3"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>43.305761316872427</v>
+      </c>
+      <c r="V12" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2678444042765005</v>
+      </c>
+      <c r="AA12" s="3"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1830,11 +1882,15 @@
       <c r="T13" s="3">
         <v>0</v>
       </c>
-      <c r="U13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1895,11 +1951,15 @@
       <c r="T14" s="3">
         <v>0</v>
       </c>
-      <c r="U14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1960,11 +2020,15 @@
       <c r="T15" s="3">
         <v>0</v>
       </c>
-      <c r="U15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2025,12 +2089,16 @@
       <c r="T16" s="3">
         <v>1102261</v>
       </c>
-      <c r="U16" s="7">
-        <f t="shared" si="0"/>
-        <v>8.4399238404335772</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U16">
+        <f t="shared" si="0"/>
+        <v>226.80267489711935</v>
+      </c>
+      <c r="V16" s="7">
+        <f t="shared" si="1"/>
+        <v>1.4293085133420678</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2091,12 +2159,16 @@
       <c r="T17" s="3">
         <v>141994</v>
       </c>
-      <c r="U17" s="7">
-        <f t="shared" si="0"/>
-        <v>10.322665589660744</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U17">
+        <f t="shared" si="0"/>
+        <v>29.216872427983539</v>
+      </c>
+      <c r="V17" s="7">
+        <f t="shared" si="1"/>
+        <v>1.7481524817796648</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2157,11 +2229,15 @@
       <c r="T18" s="3">
         <v>0</v>
       </c>
-      <c r="U18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2222,11 +2298,15 @@
       <c r="T19" s="3">
         <v>0</v>
       </c>
-      <c r="U19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2287,11 +2367,15 @@
       <c r="T20" s="3">
         <v>0</v>
       </c>
-      <c r="U20" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2352,12 +2436,16 @@
       <c r="T21" s="3">
         <v>661476</v>
       </c>
-      <c r="U21" s="7">
-        <f t="shared" si="0"/>
-        <v>8.0713982706155285</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U21">
+        <f t="shared" si="0"/>
+        <v>136.10617283950617</v>
+      </c>
+      <c r="V21" s="7">
+        <f t="shared" si="1"/>
+        <v>1.3668983844968632</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2418,11 +2506,15 @@
       <c r="T22" s="3">
         <v>0</v>
       </c>
-      <c r="U22" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2483,11 +2575,15 @@
       <c r="T23" s="3">
         <v>0</v>
       </c>
-      <c r="U23" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2548,11 +2644,15 @@
       <c r="T24" s="3">
         <v>0</v>
       </c>
-      <c r="U24" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2613,12 +2713,16 @@
       <c r="T25" s="3">
         <v>470603</v>
       </c>
-      <c r="U25" s="7">
-        <f t="shared" si="0"/>
-        <v>4.8937653095284963</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U25">
+        <f t="shared" si="0"/>
+        <v>96.83189300411523</v>
+      </c>
+      <c r="V25" s="7">
+        <f t="shared" si="1"/>
+        <v>0.82876345230715098</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2679,11 +2783,15 @@
       <c r="T26" s="3">
         <v>0</v>
       </c>
-      <c r="U26" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2744,11 +2852,15 @@
       <c r="T27" s="3">
         <v>0</v>
       </c>
-      <c r="U27" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2809,11 +2921,15 @@
       <c r="T28" s="3">
         <v>0</v>
       </c>
-      <c r="U28" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2874,11 +2990,15 @@
       <c r="T29" s="3">
         <v>0</v>
       </c>
-      <c r="U29" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2939,11 +3059,15 @@
       <c r="T30" s="3">
         <v>0</v>
       </c>
-      <c r="U30" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3004,12 +3128,16 @@
       <c r="T31" s="3">
         <v>0</v>
       </c>
-      <c r="U31" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="3"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="3"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3070,13 +3198,17 @@
       <c r="T32" s="3">
         <v>6069</v>
       </c>
-      <c r="U32" s="7">
-        <f t="shared" si="0"/>
-        <v>3.4376853146853152</v>
-      </c>
-      <c r="Z32" s="3"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U32">
+        <f t="shared" si="0"/>
+        <v>1.2487654320987653</v>
+      </c>
+      <c r="V32" s="7">
+        <f t="shared" si="1"/>
+        <v>0.58217502661947096</v>
+      </c>
+      <c r="AA32" s="3"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3137,12 +3269,16 @@
       <c r="T33" s="3">
         <v>0</v>
       </c>
-      <c r="U33" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="3"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V33" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="3"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3203,12 +3339,16 @@
       <c r="T34" s="3">
         <v>0</v>
       </c>
-      <c r="U34" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="3"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V34" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="3"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3270,13 +3410,17 @@
         <f>4698000/1000</f>
         <v>4698</v>
       </c>
-      <c r="U35" s="7">
-        <f t="shared" si="0"/>
-        <v>2.9048702290076336</v>
-      </c>
-      <c r="Z35" s="3"/>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U35">
+        <f t="shared" si="0"/>
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="V35" s="7">
+        <f t="shared" si="1"/>
+        <v>0.49194232400339266</v>
+      </c>
+      <c r="AA35" s="3"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3337,12 +3481,16 @@
       <c r="T36" s="3">
         <v>0</v>
       </c>
-      <c r="U36" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="3"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="3"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3403,12 +3551,16 @@
       <c r="T37" s="3">
         <v>0</v>
       </c>
-      <c r="U37" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="3"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V37" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="3"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3469,12 +3621,16 @@
       <c r="T38" s="3">
         <v>0</v>
       </c>
-      <c r="U38" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="3"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="3"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3535,12 +3691,16 @@
       <c r="T39" s="3">
         <v>0</v>
       </c>
-      <c r="U39" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="3"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="3"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3601,13 +3761,17 @@
       <c r="T40" s="3">
         <v>694031</v>
       </c>
-      <c r="U40" s="7">
-        <f t="shared" si="0"/>
-        <v>18.040856314584627</v>
-      </c>
-      <c r="Z40" s="3"/>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U40">
+        <f t="shared" si="0"/>
+        <v>142.80473251028806</v>
+      </c>
+      <c r="V40" s="7">
+        <f t="shared" si="1"/>
+        <v>3.0552348582676463</v>
+      </c>
+      <c r="AA40" s="3"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3668,11 +3832,15 @@
       <c r="T41" s="3">
         <v>0</v>
       </c>
-      <c r="U41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3733,11 +3901,15 @@
       <c r="T42" s="3">
         <v>0</v>
       </c>
-      <c r="U42" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3798,11 +3970,15 @@
       <c r="T43" s="3">
         <v>0</v>
       </c>
-      <c r="U43" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3863,11 +4039,15 @@
       <c r="T44" s="3">
         <v>0</v>
       </c>
-      <c r="U44" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3928,11 +4108,15 @@
       <c r="T45" s="3">
         <v>0</v>
       </c>
-      <c r="U45" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V45" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3993,12 +4177,16 @@
       <c r="T46" s="3">
         <v>0</v>
       </c>
-      <c r="U46" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="3"/>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V46" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="3"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4059,12 +4247,16 @@
       <c r="T47" s="3">
         <v>0</v>
       </c>
-      <c r="U47" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="3"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V47" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="3"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4125,11 +4317,15 @@
       <c r="T48" s="3">
         <v>0</v>
       </c>
-      <c r="U48" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V48" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4190,13 +4386,17 @@
       <c r="T49" s="3">
         <v>50700</v>
       </c>
-      <c r="U49" s="7">
-        <f>($T49*1000*$W$1)/(S49*2000)</f>
-        <v>12.097505891594659</v>
-      </c>
-      <c r="X49" s="3"/>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U49">
+        <f t="shared" si="0"/>
+        <v>10.432098765432098</v>
+      </c>
+      <c r="V49" s="7">
+        <f t="shared" si="1"/>
+        <v>2.0487232453715825</v>
+      </c>
+      <c r="Y49" s="3"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4257,11 +4457,15 @@
       <c r="T50" s="3">
         <v>0</v>
       </c>
-      <c r="U50" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V50" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4322,12 +4526,16 @@
       <c r="T51" s="3">
         <v>1075080</v>
       </c>
-      <c r="U51" s="7">
-        <f t="shared" si="0"/>
-        <v>10.801205626255861</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U51">
+        <f t="shared" si="0"/>
+        <v>221.20987654320987</v>
+      </c>
+      <c r="V51" s="7">
+        <f t="shared" si="1"/>
+        <v>1.8291936571755425</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4388,12 +4596,16 @@
       <c r="T52" s="3">
         <v>39789</v>
       </c>
-      <c r="U52" s="7">
-        <f t="shared" si="0"/>
-        <v>8.4032044150877798</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U52">
+        <f t="shared" si="0"/>
+        <v>8.1870370370370367</v>
+      </c>
+      <c r="V52" s="7">
+        <f t="shared" si="1"/>
+        <v>1.4230900464170062</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4454,13 +4666,17 @@
       <c r="T53" s="3">
         <v>51699</v>
       </c>
-      <c r="U53" s="7">
-        <f t="shared" si="0"/>
-        <v>6.6036884987384363</v>
-      </c>
-      <c r="Z53" s="3"/>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U53">
+        <f t="shared" si="0"/>
+        <v>10.637654320987654</v>
+      </c>
+      <c r="V53" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1183404458565658</v>
+      </c>
+      <c r="AA53" s="3"/>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4521,12 +4737,16 @@
       <c r="T54" s="3">
         <v>0</v>
       </c>
-      <c r="U54" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="3"/>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V54" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="3"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4587,12 +4807,16 @@
       <c r="T55" s="3">
         <v>338734</v>
       </c>
-      <c r="U55" s="7">
-        <f t="shared" si="0"/>
-        <v>10.462992500317783</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U55">
+        <f t="shared" si="0"/>
+        <v>69.698353909465027</v>
+      </c>
+      <c r="V55" s="7">
+        <f t="shared" si="1"/>
+        <v>1.771916967318292</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4653,11 +4877,15 @@
       <c r="T56" s="3">
         <v>0</v>
       </c>
-      <c r="U56" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V56" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4718,11 +4946,15 @@
       <c r="T57" s="3">
         <v>0</v>
       </c>
-      <c r="U57" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V57" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4783,12 +5015,16 @@
       <c r="T58" s="3">
         <v>98250</v>
       </c>
-      <c r="U58" s="7">
-        <f t="shared" si="0"/>
-        <v>6.4926438594582843</v>
-      </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="U58">
+        <f t="shared" si="0"/>
+        <v>20.216049382716051</v>
+      </c>
+      <c r="V58" s="7">
+        <f t="shared" si="1"/>
+        <v>1.0995349386879172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4849,80 +5085,84 @@
       <c r="T59" s="3">
         <v>5947</v>
       </c>
-      <c r="U59" s="7">
-        <f t="shared" si="0"/>
-        <v>8.8766646191646199</v>
-      </c>
-      <c r="Z59" s="3"/>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z60" s="3"/>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z61" s="3"/>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z62" s="3"/>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z63" s="3"/>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z64" s="3"/>
-    </row>
-    <row r="65" spans="26:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z65" s="3"/>
-    </row>
-    <row r="66" spans="26:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z66" s="3"/>
-    </row>
-    <row r="67" spans="26:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z67" s="3"/>
-    </row>
-    <row r="68" spans="26:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z68" s="3"/>
-    </row>
-    <row r="81" spans="26:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z81" s="3"/>
-    </row>
-    <row r="82" spans="26:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z82" s="3"/>
-    </row>
-    <row r="121" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X121" s="3"/>
-    </row>
-    <row r="122" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X122" s="3"/>
-    </row>
-    <row r="123" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X123" s="3"/>
-    </row>
-    <row r="159" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X159" s="3"/>
-    </row>
-    <row r="160" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X160" s="3"/>
-    </row>
-    <row r="161" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X161" s="3"/>
-    </row>
-    <row r="162" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X162" s="3"/>
-    </row>
-    <row r="163" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X163" s="3"/>
-    </row>
-    <row r="164" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X164" s="3"/>
-    </row>
-    <row r="165" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X165" s="3"/>
-    </row>
-    <row r="177" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X177" s="3"/>
-    </row>
-    <row r="178" spans="24:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="X178" s="3"/>
+      <c r="U59">
+        <f t="shared" si="0"/>
+        <v>1.2236625514403292</v>
+      </c>
+      <c r="V59" s="7">
+        <f t="shared" si="1"/>
+        <v>1.503270947715392</v>
+      </c>
+      <c r="AA59" s="3"/>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA60" s="3"/>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA61" s="3"/>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA62" s="3"/>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA63" s="3"/>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA64" s="3"/>
+    </row>
+    <row r="65" spans="27:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA65" s="3"/>
+    </row>
+    <row r="66" spans="27:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA66" s="3"/>
+    </row>
+    <row r="67" spans="27:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA67" s="3"/>
+    </row>
+    <row r="68" spans="27:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA68" s="3"/>
+    </row>
+    <row r="81" spans="27:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA81" s="3"/>
+    </row>
+    <row r="82" spans="27:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA82" s="3"/>
+    </row>
+    <row r="121" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y121" s="3"/>
+    </row>
+    <row r="122" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y122" s="3"/>
+    </row>
+    <row r="123" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y123" s="3"/>
+    </row>
+    <row r="159" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y159" s="3"/>
+    </row>
+    <row r="160" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y160" s="3"/>
+    </row>
+    <row r="161" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y161" s="3"/>
+    </row>
+    <row r="162" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y162" s="3"/>
+    </row>
+    <row r="163" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y163" s="3"/>
+    </row>
+    <row r="164" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y164" s="3"/>
+    </row>
+    <row r="165" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y165" s="3"/>
+    </row>
+    <row r="177" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y177" s="3"/>
+    </row>
+    <row r="178" spans="25:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y178" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
No Longer Tracking Other Commodities
Only Track Almond and removal of irrelevant code
</commit_message>
<xml_diff>
--- a/CaliforniaAlmondTracker.xlsx
+++ b/CaliforniaAlmondTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarte\Documents\Github\CMPLXSYS530\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6FE83B-3306-42F9-950F-EBF3319041D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5C7A2-5885-4123-9F90-87F16CDC7159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{924722FB-807A-4015-AC81-44A9D46CA5FA}"/>
   </bookViews>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B440007F-2E4E-4D43-9BA3-FF6B61B8A80B}">
   <dimension ref="A1:AD178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="91" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="91" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1524,7 +1524,7 @@
         <v>-121.951543</v>
       </c>
       <c r="S8" s="6">
-        <v>530</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1534,7 +1534,6 @@
         <v>0</v>
       </c>
       <c r="V8" s="7">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA8" s="3"/>

</xml_diff>